<commit_message>
add pl spreadsheet and my_notes
</commit_message>
<xml_diff>
--- a/my_patients.xlsx
+++ b/my_patients.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/Python/MyBinder/pyFHIR_models/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/Argo-PL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34879722-F292-5544-A14A-A0BA6B3C02DA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{14C52CF0-5C6B-8447-88CA-F05453B02678}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{FD5253B7-04D8-1442-A0CB-FAE4D259D958}"/>
   </bookViews>
@@ -174,18 +174,12 @@
     <t>White</t>
   </si>
   <si>
-    <t>location</t>
-  </si>
-  <si>
     <t>Queen</t>
   </si>
   <si>
     <t>St Helena</t>
   </si>
   <si>
-    <t>service</t>
-  </si>
-  <si>
     <t>proctology</t>
   </si>
   <si>
@@ -207,7 +201,13 @@
     <t>discharge_date</t>
   </si>
   <si>
-    <t>practitioner</t>
+    <t>Practitioner</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>HealthCareService</t>
   </si>
 </sst>
 </file>
@@ -249,7 +249,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -566,15 +566,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E617136-1593-F549-8B96-E485ED23CA26}">
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.6640625" customWidth="1"/>
-    <col min="17" max="17" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5" customWidth="1"/>
     <col min="18" max="18" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -619,19 +620,19 @@
         <v>12</v>
       </c>
       <c r="N1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P1" t="s">
         <v>58</v>
       </c>
-      <c r="O1" t="s">
-        <v>47</v>
-      </c>
-      <c r="P1" t="s">
-        <v>50</v>
-      </c>
       <c r="Q1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="R1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
@@ -675,21 +676,21 @@
         <v>94559</v>
       </c>
       <c r="N2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="O2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Q2" s="2">
         <f ca="1">TODAY()-1</f>
-        <v>43953</v>
+        <v>43954</v>
       </c>
       <c r="R2" s="2">
         <f ca="1">TODAY()</f>
-        <v>43954</v>
+        <v>43955</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
@@ -733,21 +734,21 @@
         <v>94558</v>
       </c>
       <c r="N3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="P3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="Q3" s="2">
         <f ca="1">TODAY()-1</f>
-        <v>43953</v>
+        <v>43954</v>
       </c>
       <c r="R3" s="2">
         <f ca="1">TODAY()</f>
-        <v>43954</v>
+        <v>43955</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
@@ -791,21 +792,21 @@
         <v>94559</v>
       </c>
       <c r="N4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="O4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="Q4" s="2">
         <f ca="1">TODAY()-1</f>
-        <v>43953</v>
+        <v>43954</v>
       </c>
       <c r="R4" s="2">
         <f ca="1">TODAY()+1</f>
-        <v>43955</v>
+        <v>43956</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
@@ -849,21 +850,21 @@
         <v>94558</v>
       </c>
       <c r="N5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O5" t="s">
+        <v>48</v>
+      </c>
+      <c r="P5" t="s">
         <v>49</v>
-      </c>
-      <c r="P5" t="s">
-        <v>51</v>
       </c>
       <c r="Q5" s="2">
         <f ca="1">TODAY()</f>
-        <v>43954</v>
+        <v>43955</v>
       </c>
       <c r="R5" s="2">
         <f ca="1">TODAY()+1</f>
-        <v>43955</v>
+        <v>43956</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
@@ -907,21 +908,21 @@
         <v>94559</v>
       </c>
       <c r="N6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="O6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="Q6" s="2">
         <f ca="1">TODAY()</f>
-        <v>43954</v>
+        <v>43955</v>
       </c>
       <c r="R6" s="2">
         <f ca="1">TODAY()+1</f>
-        <v>43955</v>
+        <v>43956</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
@@ -965,21 +966,21 @@
         <v>94558</v>
       </c>
       <c r="N7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="P7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="Q7" s="2">
         <f ca="1">TODAY()</f>
-        <v>43954</v>
+        <v>43955</v>
       </c>
       <c r="R7" s="2">
         <f ca="1">TODAY()+1</f>
-        <v>43955</v>
+        <v>43956</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
@@ -1023,21 +1024,21 @@
         <v>94558</v>
       </c>
       <c r="N8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="O8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Q8" s="2">
         <f ca="1">TODAY()</f>
-        <v>43954</v>
+        <v>43955</v>
       </c>
       <c r="R8" s="2">
         <f ca="1">TODAY()+2</f>
-        <v>43956</v>
+        <v>43957</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
@@ -1081,21 +1082,21 @@
         <v>94558</v>
       </c>
       <c r="N9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="P9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="Q9" s="2">
         <f ca="1">TODAY()+1</f>
-        <v>43955</v>
+        <v>43956</v>
       </c>
       <c r="R9" s="2">
         <f ca="1">TODAY()+3</f>
-        <v>43957</v>
+        <v>43958</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
@@ -1139,21 +1140,21 @@
         <v>94558</v>
       </c>
       <c r="N10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="O10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="Q10" s="2">
         <f ca="1">TODAY()+1</f>
-        <v>43955</v>
+        <v>43956</v>
       </c>
       <c r="R10" s="2">
         <f t="shared" ref="R10:R11" ca="1" si="0">TODAY()+2</f>
-        <v>43956</v>
+        <v>43957</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
@@ -1197,21 +1198,21 @@
         <v>94558</v>
       </c>
       <c r="N11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O11" t="s">
+        <v>48</v>
+      </c>
+      <c r="P11" t="s">
         <v>49</v>
-      </c>
-      <c r="P11" t="s">
-        <v>51</v>
       </c>
       <c r="Q11" s="2">
         <f ca="1">TODAY()+1</f>
-        <v>43955</v>
+        <v>43956</v>
       </c>
       <c r="R11" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43956</v>
+        <v>43957</v>
       </c>
     </row>
   </sheetData>

</xml_diff>